<commit_message>
New experiments on utilizing Prompt Decorators, Added Yaml file for configurations. More experimentation and results added
</commit_message>
<xml_diff>
--- a/plangen_gaia_results_with_challenger_prompt_decorder.xlsx
+++ b/plangen_gaia_results_with_challenger_prompt_decorder.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10511"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10608"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/smitpatel/Library/CloudStorage/GoogleDrive-smit1.patel@torontomu.ca/My Drive/MEng_Project/Project/plangen-main 3/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5FE78A34-E844-C34B-92FA-73B7E14867EC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17B791F8-1378-3B44-A5F5-1450F0F88998}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38400" yWindow="500" windowWidth="38400" windowHeight="21100" activeTab="3" xr2:uid="{B88D55A3-0EB1-0746-8FBA-DC165A6B7CCD}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17700" activeTab="4" xr2:uid="{B88D55A3-0EB1-0746-8FBA-DC165A6B7CCD}"/>
   </bookViews>
   <sheets>
     <sheet name="Rebase - Evaluation" sheetId="5" r:id="rId1"/>
@@ -11080,10 +11080,9 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6477E5D4-9B1C-8E40-9C53-BDE4763106B1}">
-  <sheetPr filterMode="1"/>
   <dimension ref="A1:C167"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B169" sqref="B169"/>
     </sheetView>
   </sheetViews>
@@ -11104,7 +11103,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="2" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>318</v>
       </c>
@@ -11116,7 +11115,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>156</v>
       </c>
@@ -11128,7 +11127,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>319</v>
       </c>
@@ -11140,7 +11139,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>320</v>
       </c>
@@ -11152,7 +11151,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>70</v>
       </c>
@@ -11164,7 +11163,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>321</v>
       </c>
@@ -11176,7 +11175,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>7</v>
       </c>
@@ -11188,7 +11187,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>162</v>
       </c>
@@ -11200,7 +11199,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>322</v>
       </c>
@@ -11212,7 +11211,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
         <v>323</v>
       </c>
@@ -11224,7 +11223,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
         <v>324</v>
       </c>
@@ -11236,7 +11235,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
         <v>325</v>
       </c>
@@ -11248,7 +11247,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
         <v>326</v>
       </c>
@@ -11260,7 +11259,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
         <v>327</v>
       </c>
@@ -11272,7 +11271,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
         <v>328</v>
       </c>
@@ -11284,7 +11283,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
         <v>329</v>
       </c>
@@ -11296,7 +11295,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
         <v>330</v>
       </c>
@@ -11308,7 +11307,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
         <v>331</v>
       </c>
@@ -11320,7 +11319,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
         <v>332</v>
       </c>
@@ -11332,7 +11331,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
         <v>333</v>
       </c>
@@ -11344,7 +11343,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
         <v>334</v>
       </c>
@@ -11356,7 +11355,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
         <v>335</v>
       </c>
@@ -11368,7 +11367,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="s">
         <v>336</v>
       </c>
@@ -11380,7 +11379,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A25" s="1" t="s">
         <v>337</v>
       </c>
@@ -11392,7 +11391,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A26" s="1" t="s">
         <v>338</v>
       </c>
@@ -11404,7 +11403,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A27" s="1" t="s">
         <v>3</v>
       </c>
@@ -11416,7 +11415,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A28" s="1" t="s">
         <v>339</v>
       </c>
@@ -11428,7 +11427,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A29" s="1" t="s">
         <v>340</v>
       </c>
@@ -11440,7 +11439,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A30" s="1" t="s">
         <v>341</v>
       </c>
@@ -11452,7 +11451,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A31" s="1" t="s">
         <v>167</v>
       </c>
@@ -11464,7 +11463,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A32" s="1" t="s">
         <v>342</v>
       </c>
@@ -11476,7 +11475,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A33" s="1" t="s">
         <v>343</v>
       </c>
@@ -11488,7 +11487,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A34" s="1" t="s">
         <v>242</v>
       </c>
@@ -11500,7 +11499,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A35" s="1" t="s">
         <v>344</v>
       </c>
@@ -11512,7 +11511,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A36" s="1" t="s">
         <v>345</v>
       </c>
@@ -11524,7 +11523,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A37" s="1" t="s">
         <v>7</v>
       </c>
@@ -11536,7 +11535,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A38" s="1" t="s">
         <v>346</v>
       </c>
@@ -11548,7 +11547,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A39" s="1" t="s">
         <v>347</v>
       </c>
@@ -11560,7 +11559,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A40" s="1" t="s">
         <v>348</v>
       </c>
@@ -11572,7 +11571,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A41" s="1" t="s">
         <v>349</v>
       </c>
@@ -11584,7 +11583,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A42" s="1" t="s">
         <v>15</v>
       </c>
@@ -11596,7 +11595,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A43" s="1" t="s">
         <v>350</v>
       </c>
@@ -11608,7 +11607,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A44" s="1" t="s">
         <v>351</v>
       </c>
@@ -11620,7 +11619,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A45" s="1" t="s">
         <v>352</v>
       </c>
@@ -11632,7 +11631,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A46" s="1" t="s">
         <v>353</v>
       </c>
@@ -11644,7 +11643,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A47" s="1" t="s">
         <v>167</v>
       </c>
@@ -11656,7 +11655,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A48" s="1" t="s">
         <v>354</v>
       </c>
@@ -11668,7 +11667,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A49" s="1" t="s">
         <v>355</v>
       </c>
@@ -11680,7 +11679,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A50" s="1" t="s">
         <v>11</v>
       </c>
@@ -11704,7 +11703,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="52" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A52" s="1" t="s">
         <v>357</v>
       </c>
@@ -11716,7 +11715,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="53" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A53" s="1" t="s">
         <v>358</v>
       </c>
@@ -11728,7 +11727,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A54" s="1" t="s">
         <v>170</v>
       </c>
@@ -11740,7 +11739,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="55" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A55" s="1" t="s">
         <v>359</v>
       </c>
@@ -11752,7 +11751,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="56" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A56" s="1" t="s">
         <v>360</v>
       </c>
@@ -11764,7 +11763,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="57" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A57" s="1" t="s">
         <v>361</v>
       </c>
@@ -11776,7 +11775,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="58" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A58" s="1" t="s">
         <v>49</v>
       </c>
@@ -11788,7 +11787,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="59" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A59" s="1" t="s">
         <v>362</v>
       </c>
@@ -11800,7 +11799,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="60" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A60" s="1" t="s">
         <v>363</v>
       </c>
@@ -11812,7 +11811,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="61" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A61" s="1" t="s">
         <v>364</v>
       </c>
@@ -11824,7 +11823,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="62" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A62" s="1" t="s">
         <v>11</v>
       </c>
@@ -11836,7 +11835,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="63" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A63" s="1" t="s">
         <v>12</v>
       </c>
@@ -11848,7 +11847,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="64" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A64" s="1" t="s">
         <v>6</v>
       </c>
@@ -11860,7 +11859,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="65" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A65" s="1" t="s">
         <v>11</v>
       </c>
@@ -11872,7 +11871,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="66" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A66" s="1" t="s">
         <v>329</v>
       </c>
@@ -11884,7 +11883,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="67" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A67" s="1" t="s">
         <v>365</v>
       </c>
@@ -11896,7 +11895,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="68" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A68" s="1" t="s">
         <v>50</v>
       </c>
@@ -11908,7 +11907,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="69" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A69" s="1" t="s">
         <v>366</v>
       </c>
@@ -11920,7 +11919,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="70" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A70" s="1" t="s">
         <v>367</v>
       </c>
@@ -11932,7 +11931,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="71" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A71" s="1" t="s">
         <v>368</v>
       </c>
@@ -11944,7 +11943,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="72" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A72" s="1" t="s">
         <v>369</v>
       </c>
@@ -11956,7 +11955,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="73" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A73" s="1" t="s">
         <v>370</v>
       </c>
@@ -11968,7 +11967,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="74" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A74" s="1" t="s">
         <v>371</v>
       </c>
@@ -11980,7 +11979,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="75" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A75" s="1" t="s">
         <v>372</v>
       </c>
@@ -11992,7 +11991,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="76" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A76" s="1" t="s">
         <v>373</v>
       </c>
@@ -12004,7 +12003,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="77" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A77" s="1" t="s">
         <v>374</v>
       </c>
@@ -12016,7 +12015,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="78" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A78" s="1" t="s">
         <v>375</v>
       </c>
@@ -12028,7 +12027,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="79" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A79" s="1" t="s">
         <v>329</v>
       </c>
@@ -12052,7 +12051,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="81" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A81" s="1" t="s">
         <v>11</v>
       </c>
@@ -12064,7 +12063,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="82" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A82" s="1" t="s">
         <v>376</v>
       </c>
@@ -12076,7 +12075,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="83" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A83" s="1" t="s">
         <v>2</v>
       </c>
@@ -12088,7 +12087,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="84" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A84" s="1" t="s">
         <v>156</v>
       </c>
@@ -12100,7 +12099,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="85" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A85" s="1" t="s">
         <v>2</v>
       </c>
@@ -12112,7 +12111,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="86" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A86" s="1" t="s">
         <v>377</v>
       </c>
@@ -12124,7 +12123,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="87" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A87" s="1" t="s">
         <v>49</v>
       </c>
@@ -12136,7 +12135,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="88" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A88" s="1" t="s">
         <v>378</v>
       </c>
@@ -12148,7 +12147,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="89" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A89" s="1" t="s">
         <v>379</v>
       </c>
@@ -12160,7 +12159,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="90" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A90" s="1" t="s">
         <v>380</v>
       </c>
@@ -12172,7 +12171,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="91" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A91" s="1" t="s">
         <v>13</v>
       </c>
@@ -12184,7 +12183,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="92" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A92" s="1" t="s">
         <v>381</v>
       </c>
@@ -12196,7 +12195,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="93" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A93" s="1" t="s">
         <v>382</v>
       </c>
@@ -12208,7 +12207,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="94" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A94" s="1" t="s">
         <v>383</v>
       </c>
@@ -12220,7 +12219,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="95" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A95" s="1" t="s">
         <v>384</v>
       </c>
@@ -12232,7 +12231,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="96" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A96" s="1" t="s">
         <v>385</v>
       </c>
@@ -12244,7 +12243,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="97" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A97" s="1" t="s">
         <v>386</v>
       </c>
@@ -12256,7 +12255,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="98" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A98" s="1" t="s">
         <v>62</v>
       </c>
@@ -12268,7 +12267,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="99" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A99" s="1" t="s">
         <v>387</v>
       </c>
@@ -12280,7 +12279,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="100" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A100" s="1" t="s">
         <v>388</v>
       </c>
@@ -12292,7 +12291,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="101" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A101" s="1" t="s">
         <v>389</v>
       </c>
@@ -12304,7 +12303,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="102" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A102" s="1" t="s">
         <v>390</v>
       </c>
@@ -12316,7 +12315,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="103" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A103" s="1" t="s">
         <v>391</v>
       </c>
@@ -12328,7 +12327,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="104" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A104" s="1" t="s">
         <v>392</v>
       </c>
@@ -12340,7 +12339,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="105" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A105" s="1" t="s">
         <v>393</v>
       </c>
@@ -12352,7 +12351,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="106" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A106" s="1" t="s">
         <v>394</v>
       </c>
@@ -12364,7 +12363,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="107" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A107" s="1" t="s">
         <v>395</v>
       </c>
@@ -12376,7 +12375,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="108" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="108" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A108" s="1" t="s">
         <v>396</v>
       </c>
@@ -12388,7 +12387,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="109" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="109" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A109" s="1" t="s">
         <v>397</v>
       </c>
@@ -12400,7 +12399,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="110" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="110" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A110" s="1" t="s">
         <v>398</v>
       </c>
@@ -12412,7 +12411,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="111" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="111" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A111" s="1" t="s">
         <v>7</v>
       </c>
@@ -12424,7 +12423,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="112" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="112" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A112" s="1" t="s">
         <v>399</v>
       </c>
@@ -12436,7 +12435,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="113" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="113" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A113" s="1" t="s">
         <v>68</v>
       </c>
@@ -12448,7 +12447,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="114" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="114" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A114" s="1" t="s">
         <v>400</v>
       </c>
@@ -12460,7 +12459,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="115" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="115" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A115" s="1" t="s">
         <v>401</v>
       </c>
@@ -12472,7 +12471,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="116" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="116" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A116" s="1" t="s">
         <v>402</v>
       </c>
@@ -12484,7 +12483,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="117" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="117" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A117" s="1" t="s">
         <v>403</v>
       </c>
@@ -12496,7 +12495,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="118" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="118" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A118" s="1" t="s">
         <v>404</v>
       </c>
@@ -12508,7 +12507,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="119" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="119" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A119" s="1" t="s">
         <v>405</v>
       </c>
@@ -12520,7 +12519,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="120" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="120" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A120" s="1" t="s">
         <v>11</v>
       </c>
@@ -12532,7 +12531,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="121" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="121" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A121" s="1" t="s">
         <v>279</v>
       </c>
@@ -12544,7 +12543,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="122" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="122" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A122" s="1" t="s">
         <v>406</v>
       </c>
@@ -12556,7 +12555,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="123" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="123" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A123" s="1" t="s">
         <v>407</v>
       </c>
@@ -12580,7 +12579,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="125" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="125" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A125" s="1" t="s">
         <v>192</v>
       </c>
@@ -12592,7 +12591,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="126" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="126" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A126" s="1" t="s">
         <v>408</v>
       </c>
@@ -12604,7 +12603,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="127" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="127" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A127" s="1" t="s">
         <v>191</v>
       </c>
@@ -12616,7 +12615,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="128" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="128" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A128" s="1" t="s">
         <v>409</v>
       </c>
@@ -12628,7 +12627,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="129" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="129" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A129" s="1" t="s">
         <v>410</v>
       </c>
@@ -12640,7 +12639,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="130" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="130" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A130" s="1" t="s">
         <v>411</v>
       </c>
@@ -12652,7 +12651,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="131" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="131" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A131" s="1" t="s">
         <v>412</v>
       </c>
@@ -12664,7 +12663,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="132" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="132" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A132" s="1" t="s">
         <v>413</v>
       </c>
@@ -12676,7 +12675,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="133" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="133" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A133" s="1" t="s">
         <v>414</v>
       </c>
@@ -12688,7 +12687,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="134" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="134" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A134" s="1" t="s">
         <v>415</v>
       </c>
@@ -12700,7 +12699,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="135" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="135" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A135" s="1" t="s">
         <v>416</v>
       </c>
@@ -12712,7 +12711,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="136" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="136" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A136" s="1" t="s">
         <v>417</v>
       </c>
@@ -12724,7 +12723,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="137" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="137" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A137" s="1" t="s">
         <v>418</v>
       </c>
@@ -12736,7 +12735,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="138" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="138" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A138" s="1" t="s">
         <v>419</v>
       </c>
@@ -12748,7 +12747,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="139" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="139" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A139" s="1" t="s">
         <v>420</v>
       </c>
@@ -12760,7 +12759,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="140" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="140" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A140" s="1" t="s">
         <v>7</v>
       </c>
@@ -12772,7 +12771,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="141" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="141" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A141" s="1" t="s">
         <v>421</v>
       </c>
@@ -12784,7 +12783,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="142" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="142" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A142" s="1" t="s">
         <v>422</v>
       </c>
@@ -12796,7 +12795,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="143" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="143" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A143" s="1" t="s">
         <v>423</v>
       </c>
@@ -12808,7 +12807,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="144" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="144" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A144" s="1" t="s">
         <v>145</v>
       </c>
@@ -12820,7 +12819,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="145" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="145" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A145" s="1" t="s">
         <v>267</v>
       </c>
@@ -12832,7 +12831,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="146" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="146" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A146" s="1" t="s">
         <v>424</v>
       </c>
@@ -12844,7 +12843,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="147" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="147" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A147" s="1" t="s">
         <v>425</v>
       </c>
@@ -12856,7 +12855,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="148" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="148" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A148" s="1" t="s">
         <v>426</v>
       </c>
@@ -12868,7 +12867,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="149" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="149" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A149" s="1" t="s">
         <v>11</v>
       </c>
@@ -12880,7 +12879,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="150" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="150" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A150" s="1" t="s">
         <v>427</v>
       </c>
@@ -12892,7 +12891,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="151" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="151" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A151" s="1" t="s">
         <v>428</v>
       </c>
@@ -12904,7 +12903,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="152" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="152" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A152" s="1" t="s">
         <v>198</v>
       </c>
@@ -12916,7 +12915,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="153" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="153" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A153" s="1" t="s">
         <v>429</v>
       </c>
@@ -12928,7 +12927,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="154" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="154" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A154" s="1" t="s">
         <v>430</v>
       </c>
@@ -12940,7 +12939,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="155" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="155" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A155" s="1" t="s">
         <v>431</v>
       </c>
@@ -12952,7 +12951,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="156" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="156" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A156" s="1" t="s">
         <v>432</v>
       </c>
@@ -12964,7 +12963,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="157" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="157" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A157" s="1" t="s">
         <v>433</v>
       </c>
@@ -12976,7 +12975,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="158" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="158" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A158" s="1" t="s">
         <v>434</v>
       </c>
@@ -12988,7 +12987,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="159" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="159" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A159" s="1" t="s">
         <v>435</v>
       </c>
@@ -13000,7 +12999,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="160" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="160" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A160" s="1" t="s">
         <v>436</v>
       </c>
@@ -13012,7 +13011,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="161" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="161" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A161" s="1" t="s">
         <v>437</v>
       </c>
@@ -13024,7 +13023,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="162" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="162" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A162" s="1" t="s">
         <v>438</v>
       </c>
@@ -13036,7 +13035,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="163" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="163" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A163" s="1" t="s">
         <v>22</v>
       </c>
@@ -13048,7 +13047,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="164" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="164" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A164" s="1" t="s">
         <v>21</v>
       </c>
@@ -13060,7 +13059,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="165" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="165" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A165" s="1" t="s">
         <v>167</v>
       </c>
@@ -13072,7 +13071,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="166" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="166" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A166" s="1" t="s">
         <v>439</v>
       </c>
@@ -13088,23 +13087,16 @@
       <c r="A167" s="2"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:C166" xr:uid="{6477E5D4-9B1C-8E40-9C53-BDE4763106B1}">
-    <filterColumn colId="2">
-      <filters>
-        <filter val="TRUE"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
+  <autoFilter ref="A1:C166" xr:uid="{6477E5D4-9B1C-8E40-9C53-BDE4763106B1}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E50F8EFD-8E8C-0C41-84FB-E28703B3B7F0}">
-  <sheetPr filterMode="1"/>
   <dimension ref="A1:C75"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A44" workbookViewId="0">
       <selection activeCell="A78" sqref="A78"/>
     </sheetView>
   </sheetViews>
@@ -13125,7 +13117,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="2" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>262</v>
       </c>
@@ -13137,7 +13129,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>49</v>
       </c>
@@ -13149,7 +13141,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>263</v>
       </c>
@@ -13161,7 +13153,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>264</v>
       </c>
@@ -13173,7 +13165,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>265</v>
       </c>
@@ -13185,7 +13177,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>266</v>
       </c>
@@ -13197,7 +13189,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>267</v>
       </c>
@@ -13209,7 +13201,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>268</v>
       </c>
@@ -13221,7 +13213,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>269</v>
       </c>
@@ -13233,7 +13225,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
         <v>270</v>
       </c>
@@ -13257,7 +13249,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
         <v>271</v>
       </c>
@@ -13269,7 +13261,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
         <v>9</v>
       </c>
@@ -13281,7 +13273,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
         <v>166</v>
       </c>
@@ -13293,7 +13285,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
         <v>272</v>
       </c>
@@ -13305,7 +13297,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
         <v>273</v>
       </c>
@@ -13317,7 +13309,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
         <v>274</v>
       </c>
@@ -13329,7 +13321,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
         <v>3</v>
       </c>
@@ -13341,7 +13333,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
         <v>275</v>
       </c>
@@ -13353,7 +13345,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
         <v>4</v>
       </c>
@@ -13365,7 +13357,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
         <v>276</v>
       </c>
@@ -13377,7 +13369,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
         <v>277</v>
       </c>
@@ -13389,7 +13381,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="s">
         <v>278</v>
       </c>
@@ -13401,7 +13393,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A25" s="1" t="s">
         <v>279</v>
       </c>
@@ -13413,7 +13405,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A26" s="1" t="s">
         <v>280</v>
       </c>
@@ -13425,7 +13417,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A27" s="1" t="s">
         <v>281</v>
       </c>
@@ -13437,7 +13429,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A28" s="1" t="s">
         <v>282</v>
       </c>
@@ -13449,7 +13441,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A29" s="1" t="s">
         <v>170</v>
       </c>
@@ -13461,7 +13453,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A30" s="1" t="s">
         <v>283</v>
       </c>
@@ -13473,7 +13465,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A31" s="1" t="s">
         <v>49</v>
       </c>
@@ -13485,7 +13477,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A32" s="1" t="s">
         <v>284</v>
       </c>
@@ -13497,7 +13489,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A33" s="1" t="s">
         <v>12</v>
       </c>
@@ -13509,7 +13501,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A34" s="1" t="s">
         <v>285</v>
       </c>
@@ -13521,7 +13513,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A35" s="1" t="s">
         <v>286</v>
       </c>
@@ -13533,7 +13525,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A36" s="1" t="s">
         <v>287</v>
       </c>
@@ -13545,7 +13537,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A37" s="1" t="s">
         <v>288</v>
       </c>
@@ -13557,7 +13549,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A38" s="1" t="s">
         <v>289</v>
       </c>
@@ -13569,7 +13561,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A39" s="1" t="s">
         <v>21</v>
       </c>
@@ -13581,7 +13573,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A40" s="1" t="s">
         <v>290</v>
       </c>
@@ -13593,7 +13585,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A41" s="1" t="s">
         <v>2</v>
       </c>
@@ -13617,7 +13609,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="43" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A43" s="1" t="s">
         <v>279</v>
       </c>
@@ -13641,7 +13633,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="45" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A45" s="1" t="s">
         <v>291</v>
       </c>
@@ -13653,7 +13645,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A46" s="1" t="s">
         <v>292</v>
       </c>
@@ -13665,7 +13657,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A47" s="1" t="s">
         <v>293</v>
       </c>
@@ -13677,7 +13669,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A48" s="1" t="s">
         <v>294</v>
       </c>
@@ -13689,7 +13681,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A49" s="1" t="s">
         <v>295</v>
       </c>
@@ -13701,7 +13693,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A50" s="1" t="s">
         <v>296</v>
       </c>
@@ -13713,7 +13705,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A51" s="1" t="s">
         <v>297</v>
       </c>
@@ -13725,7 +13717,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A52" s="1" t="s">
         <v>298</v>
       </c>
@@ -13737,7 +13729,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="53" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A53" s="1" t="s">
         <v>234</v>
       </c>
@@ -13749,7 +13741,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A54" s="1" t="s">
         <v>299</v>
       </c>
@@ -13761,7 +13753,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="55" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A55" s="1" t="s">
         <v>300</v>
       </c>
@@ -13773,7 +13765,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="56" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A56" s="1" t="s">
         <v>301</v>
       </c>
@@ -13785,7 +13777,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="57" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A57" s="1" t="s">
         <v>0</v>
       </c>
@@ -13797,7 +13789,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="58" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A58" s="1" t="s">
         <v>302</v>
       </c>
@@ -13809,7 +13801,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="59" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A59" s="1" t="s">
         <v>303</v>
       </c>
@@ -13821,7 +13813,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="60" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A60" s="1" t="s">
         <v>304</v>
       </c>
@@ -13833,7 +13825,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="61" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A61" s="1" t="s">
         <v>305</v>
       </c>
@@ -13845,7 +13837,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="62" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A62" s="1" t="s">
         <v>306</v>
       </c>
@@ -13857,7 +13849,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="63" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A63" s="1" t="s">
         <v>307</v>
       </c>
@@ -13869,7 +13861,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="64" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A64" s="1" t="s">
         <v>308</v>
       </c>
@@ -13881,7 +13873,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="65" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A65" s="1" t="s">
         <v>309</v>
       </c>
@@ -13893,7 +13885,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="66" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A66" s="1" t="s">
         <v>310</v>
       </c>
@@ -13905,7 +13897,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="67" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A67" s="1" t="s">
         <v>78</v>
       </c>
@@ -13917,7 +13909,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="68" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A68" s="1" t="s">
         <v>311</v>
       </c>
@@ -13929,7 +13921,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="69" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A69" s="1" t="s">
         <v>312</v>
       </c>
@@ -13941,7 +13933,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="70" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A70" s="1" t="s">
         <v>5</v>
       </c>
@@ -13953,7 +13945,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="71" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A71" s="1" t="s">
         <v>313</v>
       </c>
@@ -13965,7 +13957,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="72" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A72" s="1" t="s">
         <v>22</v>
       </c>
@@ -13977,7 +13969,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="73" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A73" s="1" t="s">
         <v>20</v>
       </c>
@@ -13989,7 +13981,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="74" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A74" s="1" t="s">
         <v>314</v>
       </c>
@@ -14001,18 +13993,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="75" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A75" s="2"/>
       <c r="B75" s="2"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:C75" xr:uid="{E50F8EFD-8E8C-0C41-84FB-E28703B3B7F0}">
-    <filterColumn colId="2">
-      <filters>
-        <filter val="TRUE"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
+  <autoFilter ref="A1:C75" xr:uid="{E50F8EFD-8E8C-0C41-84FB-E28703B3B7F0}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>